<commit_message>
atualização de dados e gráficos de séries temporais
</commit_message>
<xml_diff>
--- a/v2022/dados/dados-originais/tab_ufs.xlsx
+++ b/v2022/dados/dados-originais/tab_ufs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tchiluanda/Documents/GitHub/estatais-estados-2020/dados/dados-originais/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4ee191bcf7480867/Documentos/Github/estatais-estados-master/estatais-estados-master/v2022/dados/dados-originais/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F28A6AC0-98FA-484B-98F6-08DB8A0AC2AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{F28A6AC0-98FA-484B-98F6-08DB8A0AC2AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7DB8D68C-30EF-4AC4-9041-49F8DB39C5C8}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24240" windowHeight="13140" xr2:uid="{06E5B434-546D-441A-8AD3-4681C62FB42B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{06E5B434-546D-441A-8AD3-4681C62FB42B}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -192,9 +192,6 @@
     <t>Bahia</t>
   </si>
   <si>
-    <t>Minas gerais</t>
-  </si>
-  <si>
     <t>Espiríto Santo</t>
   </si>
   <si>
@@ -223,6 +220,9 @@
   </si>
   <si>
     <t>Distrito Federal</t>
+  </si>
+  <si>
+    <t>Minas Gerais</t>
   </si>
 </sst>
 </file>
@@ -577,18 +577,18 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.83203125" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -605,7 +605,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11</v>
       </c>
@@ -622,7 +622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>12</v>
       </c>
@@ -639,7 +639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>13</v>
       </c>
@@ -656,7 +656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>14</v>
       </c>
@@ -673,7 +673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>15</v>
       </c>
@@ -690,7 +690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>16</v>
       </c>
@@ -707,7 +707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>17</v>
       </c>
@@ -724,7 +724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>21</v>
       </c>
@@ -741,7 +741,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>22</v>
       </c>
@@ -758,7 +758,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>23</v>
       </c>
@@ -775,7 +775,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>24</v>
       </c>
@@ -792,7 +792,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>25</v>
       </c>
@@ -809,7 +809,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>26</v>
       </c>
@@ -826,7 +826,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>27</v>
       </c>
@@ -843,7 +843,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>28</v>
       </c>
@@ -860,7 +860,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>29</v>
       </c>
@@ -877,7 +877,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>31</v>
       </c>
@@ -885,7 +885,7 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="D18" t="s">
         <v>32</v>
@@ -894,7 +894,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>32</v>
       </c>
@@ -902,7 +902,7 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D19" t="s">
         <v>32</v>
@@ -911,7 +911,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>33</v>
       </c>
@@ -919,7 +919,7 @@
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D20" t="s">
         <v>32</v>
@@ -928,7 +928,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>35</v>
       </c>
@@ -936,7 +936,7 @@
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D21" t="s">
         <v>32</v>
@@ -945,7 +945,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>41</v>
       </c>
@@ -953,7 +953,7 @@
         <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D22" t="s">
         <v>33</v>
@@ -962,7 +962,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>42</v>
       </c>
@@ -970,7 +970,7 @@
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D23" t="s">
         <v>33</v>
@@ -979,7 +979,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>43</v>
       </c>
@@ -987,7 +987,7 @@
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D24" t="s">
         <v>33</v>
@@ -996,7 +996,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>50</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D25" t="s">
         <v>34</v>
@@ -1013,7 +1013,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>51</v>
       </c>
@@ -1021,7 +1021,7 @@
         <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D26" t="s">
         <v>34</v>
@@ -1030,7 +1030,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>52</v>
       </c>
@@ -1038,7 +1038,7 @@
         <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D27" t="s">
         <v>34</v>
@@ -1047,7 +1047,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>53</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D28" t="s">
         <v>34</v>

</xml_diff>